<commit_message>
A new class has been added to check push of new additions
Verification data has been updated in all the 3 test scripts
</commit_message>
<xml_diff>
--- a/MavenVtigerFW/src/test/resources/TestData.xlsx
+++ b/MavenVtigerFW/src/test/resources/TestData.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C4B3F493-2F0F-428D-8997-58C56B529C33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\selenium\DataStorage\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7EF2A6C-2FA5-44FC-B6B5-CBE7AF9427D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="19460" windowHeight="11060" activeTab="2" xr2:uid="{99068DFA-36C0-4491-9585-15A130C15366}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{99068DFA-36C0-4491-9585-15A130C15366}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -13,8 +18,7 @@
     <sheet name="OrganizationData" sheetId="3" r:id="rId3"/>
     <sheet name="ProductData" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:H17"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -56,12 +60,51 @@
     <t>Company Name</t>
   </si>
   <si>
+    <t>Rathod</t>
+  </si>
+  <si>
+    <t>LG</t>
+  </si>
+  <si>
+    <t>Organization Name</t>
+  </si>
+  <si>
+    <t>Organization Success Message</t>
+  </si>
+  <si>
+    <t>Lead Success Message</t>
+  </si>
+  <si>
+    <t>RedChip</t>
+  </si>
+  <si>
+    <t>Create Organization With Mandatory Fields</t>
+  </si>
+  <si>
+    <t>Create Of Lead With Mandatory Fields</t>
+  </si>
+  <si>
+    <t>Create Product With Mandatory Fields</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Product Success Message</t>
+  </si>
+  <si>
+    <t>Sanitizer</t>
+  </si>
+  <si>
+    <t>Lead Information</t>
+  </si>
+  <si>
     <r>
-      <t>Lead Information</t>
+      <t>Product Information</t>
     </r>
     <r>
       <rPr>
-        <sz val="6"/>
+        <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -70,45 +113,12 @@
     </r>
   </si>
   <si>
-    <t>Rathod</t>
-  </si>
-  <si>
-    <t>LG</t>
-  </si>
-  <si>
-    <t>Organization Name</t>
-  </si>
-  <si>
-    <t>Organization Success Message</t>
-  </si>
-  <si>
-    <t>Lead Success Message</t>
-  </si>
-  <si>
-    <t>RedChip</t>
-  </si>
-  <si>
-    <t>Create Organization With Mandatory Fields</t>
-  </si>
-  <si>
-    <t>Create Of Lead With Mandatory Fields</t>
-  </si>
-  <si>
-    <t>Create Product With Mandatory Fields</t>
-  </si>
-  <si>
-    <t>Product Name</t>
-  </si>
-  <si>
-    <t>Product Success Message</t>
-  </si>
-  <si>
     <r>
-      <t>Product Information</t>
+      <t>Organization Information</t>
     </r>
     <r>
       <rPr>
-        <sz val="6"/>
+        <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -116,18 +126,12 @@
       <t>  </t>
     </r>
   </si>
-  <si>
-    <t>Sanitizer</t>
-  </si>
-  <si>
-    <t>Organization Information</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +141,18 @@
     </font>
     <font>
       <sz val="6"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -162,9 +178,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,10 +539,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF46418B-A52E-44A3-A877-2C1438337E00}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -549,22 +567,25 @@
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="D3" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -576,7 +597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C84FB697-B845-447C-823B-A585D0173122}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -597,20 +618,20 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -625,7 +646,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="A1:XFD1048576"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -643,21 +664,21 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>